<commit_message>
fixing issues from management
</commit_message>
<xml_diff>
--- a/public/data/data_statistics/economics/Economic_Statistics_National_Account.xlsx
+++ b/public/data/data_statistics/economics/Economic_Statistics_National_Account.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahmedsalim/Documents/GSS Office/Apps/Web Apps/frontend/statsghana_website/public/data/data_statistics/economics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22F008E-01A5-624D-BF67-3C5F8183BD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD1C061-7635-7740-991B-2500C9ADEDBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="17680" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AnnualGDPbyExpenditureApproach" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="338">
   <si>
     <t>ID</t>
   </si>
@@ -367,15 +367,6 @@
     <t>BD21</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Type(Quarterly/ Annual)</t>
-  </si>
-  <si>
-    <t>Quarter</t>
-  </si>
-  <si>
     <t>QGDPE_Expenditure Approach_December 2025_GSS</t>
   </si>
   <si>
@@ -769,15 +760,6 @@
     <t>IM45</t>
   </si>
   <si>
-    <t xml:space="preserve">                                    Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                        Month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         YEAR</t>
-  </si>
-  <si>
     <t>MIEG September 2025 Bulletin</t>
   </si>
   <si>
@@ -800,15 +782,6 @@
   </si>
   <si>
     <t>MIEG_User Guide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                       Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                     Month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            Year</t>
   </si>
   <si>
     <t>Rebased GDP Quarterly Bullettin_2006_2025Q3_Edition _GSS</t>
@@ -1046,40 +1019,34 @@
     <t>Others</t>
   </si>
   <si>
-    <t xml:space="preserve">Category </t>
-  </si>
-  <si>
-    <t>Annual GDP By Expenditure Approach</t>
-  </si>
-  <si>
-    <t>Annual GDP By Production Approach</t>
-  </si>
-  <si>
-    <t>Quarterly GDP By Expenditure Approach</t>
-  </si>
-  <si>
     <t>Sources And Methods</t>
   </si>
   <si>
     <t>Supply and Use Tables</t>
   </si>
   <si>
-    <t>Annual GDP News Letters</t>
-  </si>
-  <si>
     <t>GDP Infographics</t>
   </si>
   <si>
     <t>Gross National Income</t>
   </si>
   <si>
-    <t>Quarterly GDP News Letter</t>
-  </si>
-  <si>
-    <t>Monthly Indicator of Economic Growth</t>
-  </si>
-  <si>
-    <t>Quarterly GDP by Production Approach</t>
+    <t>GDP By Expenditure Approach</t>
+  </si>
+  <si>
+    <t>GDP By Production Approach</t>
+  </si>
+  <si>
+    <t>GDP News Letters</t>
+  </si>
+  <si>
+    <t>GDP News Letter</t>
+  </si>
+  <si>
+    <t>MIEG</t>
+  </si>
+  <si>
+    <t>GDP by Production Approach</t>
   </si>
 </sst>
 </file>
@@ -1395,7 +1362,7 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView zoomScale="174" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1412,10 +1379,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1438,7 +1405,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -1455,7 +1422,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
@@ -1472,7 +1439,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
@@ -1489,7 +1456,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>8</v>
@@ -1506,7 +1473,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>8</v>
@@ -1523,7 +1490,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>8</v>
@@ -1540,7 +1507,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>8</v>
@@ -1557,7 +1524,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>8</v>
@@ -1577,7 +1544,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>8</v>
@@ -1594,7 +1561,7 @@
         <v>22</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>8</v>
@@ -1611,7 +1578,7 @@
         <v>25</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>8</v>
@@ -1631,7 +1598,7 @@
         <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>8</v>
@@ -1651,7 +1618,7 @@
         <v>29</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>8</v>
@@ -1671,7 +1638,7 @@
         <v>18</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>8</v>
@@ -1691,7 +1658,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>8</v>
@@ -1711,7 +1678,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>8</v>
@@ -1731,7 +1698,7 @@
         <v>36</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>8</v>
@@ -1751,7 +1718,7 @@
         <v>39</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>8</v>
@@ -1771,7 +1738,7 @@
         <v>36</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>8</v>
@@ -1871,10 +1838,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1882,177 +1849,180 @@
     <col min="2" max="2" width="46.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="C1" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F2" s="1">
         <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F3" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F4" s="1">
         <v>2012</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F5" s="1">
         <v>2011</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F6" s="1">
         <v>2013</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F7" s="1">
         <v>2014</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F8" s="1">
         <v>2012</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F9" s="1">
         <v>2011</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F10" s="1">
         <v>2012</v>
@@ -2087,13 +2057,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -2107,19 +2077,19 @@
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F2" s="1">
         <v>2025</v>
@@ -2130,19 +2100,19 @@
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F3" s="1">
         <v>2025</v>
@@ -2153,19 +2123,19 @@
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F4" s="1">
         <v>2025</v>
@@ -2176,19 +2146,19 @@
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F5" s="1">
         <v>2025</v>
@@ -2199,19 +2169,19 @@
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F6" s="1">
         <v>2024</v>
@@ -2222,19 +2192,19 @@
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F7" s="1">
         <v>2024</v>
@@ -2245,19 +2215,19 @@
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F8" s="1">
         <v>2024</v>
@@ -2268,19 +2238,19 @@
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F9" s="1">
         <v>2024</v>
@@ -2291,19 +2261,19 @@
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F10" s="1">
         <v>2023</v>
@@ -2314,19 +2284,19 @@
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F11" s="1">
         <v>2023</v>
@@ -2335,19 +2305,19 @@
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F12" s="1">
         <v>2023</v>
@@ -2358,19 +2328,19 @@
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F13" s="1">
         <v>2023</v>
@@ -2381,19 +2351,19 @@
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F14" s="1">
         <v>2022</v>
@@ -2404,19 +2374,19 @@
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F15" s="1">
         <v>2022</v>
@@ -2427,19 +2397,19 @@
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F16" s="1">
         <v>2022</v>
@@ -2450,19 +2420,19 @@
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F17" s="1">
         <v>2021</v>
@@ -2473,19 +2443,19 @@
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F18" s="1">
         <v>2021</v>
@@ -2496,19 +2466,19 @@
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F19" s="1">
         <v>2021</v>
@@ -2519,19 +2489,19 @@
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F20" s="1">
         <v>2020</v>
@@ -2542,19 +2512,19 @@
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F21" s="1">
         <v>2020</v>
@@ -2565,19 +2535,19 @@
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F22" s="1">
         <v>2020</v>
@@ -2585,19 +2555,19 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F23" s="1">
         <v>2020</v>
@@ -2608,19 +2578,19 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F24" s="1">
         <v>2019</v>
@@ -2631,19 +2601,19 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F25" s="1">
         <v>2019</v>
@@ -2651,19 +2621,19 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F26" s="1">
         <v>2019</v>
@@ -2674,19 +2644,19 @@
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F27" s="1">
         <v>2018</v>
@@ -2697,19 +2667,19 @@
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F28" s="1">
         <v>2018</v>
@@ -2717,19 +2687,19 @@
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F29" s="1">
         <v>2014</v>
@@ -2740,19 +2710,19 @@
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F30" s="1">
         <v>2013</v>
@@ -2763,19 +2733,19 @@
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F31" s="1">
         <v>2014</v>
@@ -2786,19 +2756,19 @@
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F32" s="1">
         <v>2014</v>
@@ -2809,19 +2779,19 @@
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F33" s="1">
         <v>2012</v>
@@ -2832,19 +2802,19 @@
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F34" s="1">
         <v>2011</v>
@@ -2855,19 +2825,19 @@
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F35" s="1">
         <v>2012</v>
@@ -2878,19 +2848,19 @@
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F36" s="1">
         <v>2013</v>
@@ -2901,19 +2871,19 @@
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F37" s="1">
         <v>2013</v>
@@ -2924,19 +2894,19 @@
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F38" s="1">
         <v>2012</v>
@@ -2947,19 +2917,19 @@
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F39" s="1">
         <v>2013</v>
@@ -2970,19 +2940,19 @@
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F40" s="1">
         <v>2011</v>
@@ -2993,19 +2963,19 @@
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F41" s="1">
         <v>2012</v>
@@ -3016,19 +2986,19 @@
     </row>
     <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F42" s="1">
         <v>2011</v>
@@ -3039,19 +3009,19 @@
     </row>
     <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F43" s="1">
         <v>2015</v>
@@ -3059,19 +3029,19 @@
     </row>
     <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F44" s="1">
         <v>2016</v>
@@ -3079,19 +3049,19 @@
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F45" s="1">
         <v>2014</v>
@@ -3099,19 +3069,19 @@
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>68</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F46" s="1">
         <v>2016</v>
@@ -3130,7 +3100,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C11"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3140,28 +3110,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3170,13 +3140,13 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F2" s="1">
         <v>2025</v>
@@ -3187,13 +3157,13 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F3" s="1">
         <v>2025</v>
@@ -3204,13 +3174,13 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F4" s="1">
         <v>2025</v>
@@ -3221,13 +3191,13 @@
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F5" s="1">
         <v>2025</v>
@@ -3238,13 +3208,13 @@
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F6" s="1">
         <v>2025</v>
@@ -3255,13 +3225,13 @@
         <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F7" s="1">
         <v>2025</v>
@@ -3272,13 +3242,13 @@
         <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F8" s="1">
         <v>2025</v>
@@ -3289,13 +3259,13 @@
         <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F9" s="1">
         <v>2025</v>
@@ -3306,13 +3276,13 @@
         <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F10" s="1">
         <v>2025</v>
@@ -3323,13 +3293,13 @@
         <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F11" s="1">
         <v>2025</v>
@@ -3347,8 +3317,8 @@
   </sheetPr>
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3358,28 +3328,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3388,16 +3358,16 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="F2" s="1">
         <v>2025</v>
@@ -3409,16 +3379,16 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="F3" s="1">
         <v>2025</v>
@@ -3430,16 +3400,16 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="F4" s="1">
         <v>2025</v>
@@ -3451,16 +3421,16 @@
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F5" s="1">
         <v>2025</v>
@@ -3472,16 +3442,16 @@
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F6" s="1">
         <v>2025</v>
@@ -3493,16 +3463,16 @@
         <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F7" s="1">
         <v>2024</v>
@@ -3514,16 +3484,16 @@
         <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F8" s="1">
         <v>2023</v>
@@ -3535,16 +3505,16 @@
         <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F9" s="1">
         <v>2024</v>
@@ -3556,14 +3526,14 @@
         <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F10" s="1">
         <v>2024</v>
@@ -3575,16 +3545,16 @@
         <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F11" s="1">
         <v>2024</v>
@@ -3596,16 +3566,16 @@
         <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F12" s="1">
         <v>2024</v>
@@ -3617,16 +3587,16 @@
         <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F13" s="1">
         <v>2024</v>
@@ -3638,16 +3608,16 @@
         <v>28</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="F14" s="1">
         <v>2024</v>
@@ -3659,16 +3629,16 @@
         <v>30</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F15" s="1">
         <v>2024</v>
@@ -3680,14 +3650,14 @@
         <v>31</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F16" s="1">
         <v>2023</v>
@@ -3699,14 +3669,14 @@
         <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F17" s="1">
         <v>2023</v>
@@ -3718,16 +3688,16 @@
         <v>35</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="F18" s="1">
         <v>2023</v>
@@ -3739,16 +3709,16 @@
         <v>38</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="F19" s="1">
         <v>2023</v>
@@ -3760,16 +3730,16 @@
         <v>41</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F20" s="1">
         <v>2023</v>
@@ -3781,16 +3751,16 @@
         <v>42</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F21" s="1">
         <v>2023</v>
@@ -3802,16 +3772,16 @@
         <v>43</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F22" s="1">
         <v>2023</v>
@@ -3823,16 +3793,16 @@
         <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F23" s="1">
         <v>2023</v>
@@ -3844,16 +3814,16 @@
         <v>45</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F24" s="1">
         <v>2023</v>
@@ -3865,16 +3835,16 @@
         <v>46</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F25" s="1">
         <v>2022</v>
@@ -3886,16 +3856,16 @@
         <v>47</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F26" s="1">
         <v>2023</v>
@@ -3907,16 +3877,16 @@
         <v>48</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="F27" s="1">
         <v>2023</v>
@@ -3928,16 +3898,16 @@
         <v>49</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F28" s="1">
         <v>2023</v>
@@ -3949,16 +3919,16 @@
         <v>50</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="F29" s="1">
         <v>2023</v>
@@ -3970,16 +3940,16 @@
         <v>51</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F30" s="1">
         <v>2022</v>
@@ -3991,16 +3961,16 @@
         <v>52</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="F31" s="1">
         <v>2022</v>
@@ -4012,16 +3982,16 @@
         <v>53</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F32" s="1">
         <v>2022</v>
@@ -4033,16 +4003,16 @@
         <v>54</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F33" s="1">
         <v>2022</v>
@@ -4054,16 +4024,16 @@
         <v>55</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="F34" s="1">
         <v>2022</v>
@@ -4075,16 +4045,16 @@
         <v>56</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F35" s="1">
         <v>2022</v>
@@ -4096,16 +4066,16 @@
         <v>57</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F36" s="1">
         <v>2022</v>
@@ -4117,16 +4087,16 @@
         <v>58</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F37" s="1">
         <v>2022</v>
@@ -4138,14 +4108,14 @@
         <v>59</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="F38" s="1">
         <v>2022</v>
@@ -4157,16 +4127,16 @@
         <v>60</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="F39" s="1">
         <v>2022</v>
@@ -4178,16 +4148,16 @@
         <v>61</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F40" s="1">
         <v>2021</v>
@@ -4199,16 +4169,16 @@
         <v>62</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F41" s="1">
         <v>2021</v>
@@ -4220,16 +4190,16 @@
         <v>63</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="F42" s="1">
         <v>2021</v>
@@ -4241,16 +4211,16 @@
         <v>64</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F43" s="1">
         <v>2021</v>
@@ -4262,16 +4232,16 @@
         <v>65</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F44" s="1">
         <v>2020</v>
@@ -4280,19 +4250,19 @@
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="F45" s="1">
         <v>2020</v>
@@ -4301,19 +4271,19 @@
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F46" s="1">
         <v>2020</v>
@@ -4322,19 +4292,19 @@
     </row>
     <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="F47" s="1">
         <v>2020</v>
@@ -4343,19 +4313,19 @@
     </row>
     <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="F48" s="1">
         <v>2019</v>
@@ -4364,19 +4334,19 @@
     </row>
     <row r="49" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="F49" s="1">
         <v>2019</v>
@@ -4385,19 +4355,19 @@
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F50" s="1">
         <v>2019</v>
@@ -4406,19 +4376,19 @@
     </row>
     <row r="51" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F51" s="1">
         <v>2019</v>
@@ -4427,19 +4397,19 @@
     </row>
     <row r="52" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F52" s="1">
         <v>2019</v>
@@ -4448,19 +4418,19 @@
     </row>
     <row r="53" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F53" s="1">
         <v>2019</v>
@@ -4469,19 +4439,19 @@
     </row>
     <row r="54" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="F54" s="1">
         <v>2018</v>
@@ -4490,19 +4460,19 @@
     </row>
     <row r="55" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="F55" s="1">
         <v>2012</v>
@@ -4511,17 +4481,17 @@
     </row>
     <row r="56" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="4" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="F56" s="1">
         <v>2012</v>
@@ -4532,17 +4502,17 @@
     </row>
     <row r="57" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="4" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="F57" s="1">
         <v>2012</v>
@@ -4553,19 +4523,19 @@
     </row>
     <row r="58" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F58" s="1">
         <v>2014</v>
@@ -4574,40 +4544,40 @@
     </row>
     <row r="59" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="F59" s="1">
         <v>2013</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="F60" s="1">
         <v>2015</v>
@@ -4616,19 +4586,19 @@
     </row>
     <row r="61" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F61" s="1">
         <v>2015</v>
@@ -4637,19 +4607,19 @@
     </row>
     <row r="62" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F62" s="1">
         <v>2016</v>
@@ -9358,7 +9328,7 @@
   </sheetPr>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="231" workbookViewId="0">
+    <sheetView zoomScale="231" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C22"/>
     </sheetView>
   </sheetViews>
@@ -9377,10 +9347,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>66</v>
@@ -9403,7 +9373,7 @@
         <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -9420,7 +9390,7 @@
         <v>73</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
@@ -9437,7 +9407,7 @@
         <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
@@ -9454,7 +9424,7 @@
         <v>77</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>8</v>
@@ -9471,7 +9441,7 @@
         <v>79</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>8</v>
@@ -9488,7 +9458,7 @@
         <v>81</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>8</v>
@@ -9505,7 +9475,7 @@
         <v>83</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>68</v>
@@ -9525,7 +9495,7 @@
         <v>85</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>8</v>
@@ -9542,7 +9512,7 @@
         <v>87</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>8</v>
@@ -9559,7 +9529,7 @@
         <v>89</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>8</v>
@@ -9579,7 +9549,7 @@
         <v>91</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>8</v>
@@ -9599,7 +9569,7 @@
         <v>93</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>8</v>
@@ -9616,7 +9586,7 @@
         <v>95</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>8</v>
@@ -9633,7 +9603,7 @@
         <v>97</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>8</v>
@@ -9650,7 +9620,7 @@
         <v>99</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>68</v>
@@ -9670,7 +9640,7 @@
         <v>101</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>68</v>
@@ -9690,7 +9660,7 @@
         <v>103</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>68</v>
@@ -9710,7 +9680,7 @@
         <v>105</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>68</v>
@@ -9730,7 +9700,7 @@
         <v>107</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>8</v>
@@ -9750,7 +9720,7 @@
         <v>109</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>8</v>
@@ -9770,7 +9740,7 @@
         <v>107</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>8</v>
@@ -9792,10 +9762,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="233" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C12"/>
+    <sheetView zoomScale="233" workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9805,244 +9775,247 @@
     <col min="4" max="4" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>68</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F2" s="1">
         <v>2025</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>68</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F3" s="1">
         <v>2025</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>68</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F4" s="1">
         <v>2025</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>68</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F5" s="1">
         <v>2025</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>68</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F6" s="1">
         <v>2024</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>68</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F7" s="1">
         <v>2024</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>68</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F8" s="1">
         <v>2024</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>68</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F9" s="1">
         <v>2024</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>68</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F10" s="1">
         <v>2023</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>68</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F11" s="1">
         <v>2023</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>68</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F12" s="1">
         <v>2023</v>
@@ -10061,7 +10034,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10072,29 +10045,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>69</v>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10102,13 +10075,13 @@
         <v>70</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F2" s="1">
         <v>2019</v>
@@ -10119,13 +10092,13 @@
         <v>72</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F3" s="1">
         <v>2017</v>
@@ -10136,13 +10109,13 @@
         <v>74</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F4" s="1">
         <v>2007</v>
@@ -10164,7 +10137,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10175,29 +10148,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>69</v>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10205,14 +10178,14 @@
         <v>70</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F2" s="1">
         <v>2023</v>
@@ -10231,7 +10204,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10242,29 +10215,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>69</v>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10272,14 +10245,14 @@
         <v>70</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F2" s="1">
         <v>2020</v>
@@ -10298,7 +10271,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C8"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10307,44 +10280,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="C1" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F2" s="1">
         <v>2020</v>
@@ -10352,16 +10325,16 @@
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F3" s="1">
         <v>2018</v>
@@ -10369,16 +10342,16 @@
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F4" s="1">
         <v>2013</v>
@@ -10386,16 +10359,16 @@
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F5" s="1">
         <v>2012</v>
@@ -10403,16 +10376,16 @@
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F6" s="1">
         <v>2008</v>
@@ -10420,16 +10393,16 @@
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F7" s="1">
         <v>2015</v>
@@ -10437,16 +10410,16 @@
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F8" s="1">
         <v>2014</v>
@@ -10465,7 +10438,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10475,43 +10448,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="C1" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F2" s="1">
         <v>2025</v>
@@ -10519,16 +10492,16 @@
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F3" s="1">
         <v>2025</v>
@@ -10536,16 +10509,16 @@
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F4" s="1">
         <v>2025</v>
@@ -10582,13 +10555,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -10602,16 +10575,16 @@
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F2" s="1">
         <v>2025</v>
@@ -10619,16 +10592,16 @@
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F3" s="1">
         <v>2024</v>
@@ -10636,16 +10609,16 @@
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>79</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F4" s="1">
         <v>2023</v>
@@ -10653,16 +10626,16 @@
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F5" s="1">
         <v>2023</v>
@@ -10670,16 +10643,16 @@
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F6" s="1">
         <v>2012</v>
@@ -10687,16 +10660,16 @@
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F7" s="1">
         <v>2013</v>
@@ -10704,16 +10677,16 @@
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F8" s="1">
         <v>2012</v>
@@ -10721,16 +10694,16 @@
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F9" s="1">
         <v>2011</v>

</xml_diff>